<commit_message>
medicine-print: reorder columns to 번호-약품명-약품코드-유효기간
</commit_message>
<xml_diff>
--- a/exports/medicine-print-range-split-7.5cm.xlsx
+++ b/exports/medicine-print-range-split-7.5cm.xlsx
@@ -26,1153 +26,1153 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="383">
   <si>
+    <t>번호</t>
+  </si>
+  <si>
+    <t>약품명</t>
+  </si>
+  <si>
     <t>약품코드</t>
   </si>
   <si>
-    <t>약품명</t>
-  </si>
-  <si>
-    <t>번호</t>
-  </si>
-  <si>
     <t>유효기간</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>발트렉스정500mg</t>
+  </si>
+  <si>
     <t>vacv</t>
   </si>
   <si>
-    <t>발트렉스정500mg</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>리포덱스450mg</t>
+  </si>
+  <si>
     <t>rf45</t>
   </si>
   <si>
-    <t>리포덱스450mg</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>기넥신에프정</t>
   </si>
   <si>
     <t>gkb</t>
   </si>
   <si>
-    <t>기넥신에프정</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>46367</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>디튜린정0.1mg</t>
+  </si>
+  <si>
     <t>dsmp0.1</t>
   </si>
   <si>
-    <t>디튜린정0.1mg</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>46794</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>큐티핀정25mg</t>
+  </si>
+  <si>
     <t>quet1</t>
   </si>
   <si>
-    <t>큐티핀정25mg</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>46907</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>칼디플러스</t>
+  </si>
+  <si>
     <t>cald1</t>
   </si>
   <si>
-    <t>칼디플러스</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>46936</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>클래리시드엑스엘</t>
+  </si>
+  <si>
     <t>cltm50</t>
   </si>
   <si>
-    <t>클래리시드엑스엘</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>애피언트10mg</t>
   </si>
   <si>
     <t>effi</t>
   </si>
   <si>
-    <t>애피언트10mg</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>바난정(씨제이)</t>
   </si>
   <si>
     <t>bann</t>
   </si>
   <si>
-    <t>바난정(씨제이)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>46859</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>쿠에타핀 정 12.5mg</t>
+  </si>
+  <si>
     <t>quet0.5</t>
   </si>
   <si>
-    <t>쿠에타핀 정 12.5mg</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>46937</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>모록사신400mg</t>
+  </si>
+  <si>
     <t>avlx3</t>
   </si>
   <si>
-    <t>모록사신400mg</t>
-  </si>
-  <si>
-    <t>13</t>
+    <t>14</t>
+  </si>
+  <si>
+    <t>일성이솦틴서방정180mg</t>
   </si>
   <si>
     <t>vpm</t>
   </si>
   <si>
-    <t>일성이솦틴서방정180mg</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>후라시닐정</t>
   </si>
   <si>
     <t>fla</t>
   </si>
   <si>
-    <t>후라시닐정</t>
-  </si>
-  <si>
-    <t>15</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>테놀민정50mg</t>
   </si>
   <si>
     <t>atn50</t>
   </si>
   <si>
-    <t>테놀민정50mg</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>46793</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>아디팜정</t>
+  </si>
+  <si>
     <t>hoz</t>
   </si>
   <si>
-    <t>아디팜정</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>메섹신캅셀500mg</t>
   </si>
   <si>
     <t>msx1</t>
   </si>
   <si>
-    <t>메섹신캅셀500mg</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>46380</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>다이아벡스정1000mg</t>
+  </si>
+  <si>
     <t>gph10</t>
   </si>
   <si>
-    <t>다이아벡스정1000mg</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>46726</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>글리멜정2mg</t>
+  </si>
+  <si>
     <t>glmp</t>
   </si>
   <si>
-    <t>글리멜정2mg</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>디오살탄정40mg</t>
   </si>
   <si>
     <t>dio40</t>
   </si>
   <si>
-    <t>디오살탄정40mg</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>46814</t>
   </si>
   <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>리록스반정15mg</t>
+  </si>
+  <si>
     <t>xarel15</t>
   </si>
   <si>
-    <t>리록스반정15mg</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>46477</t>
   </si>
   <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>엘탄 서방정 60mg</t>
+  </si>
+  <si>
     <t>isod1</t>
   </si>
   <si>
-    <t>엘탄 서방정 60mg</t>
-  </si>
-  <si>
-    <t>25</t>
+    <t>26</t>
+  </si>
+  <si>
+    <t>다이아벡스XR서방정</t>
   </si>
   <si>
     <t>gph-xr</t>
   </si>
   <si>
-    <t>다이아벡스XR서방정</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>46631</t>
   </si>
   <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>아토르바10mg</t>
+  </si>
+  <si>
     <t>lipi10</t>
   </si>
   <si>
-    <t>아토르바10mg</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>46507</t>
   </si>
   <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>판토라인20mg</t>
+  </si>
+  <si>
     <t>ptp2</t>
   </si>
   <si>
-    <t>판토라인20mg</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>46732</t>
   </si>
   <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>엘리퀴스정2.5mg</t>
+  </si>
+  <si>
     <t>eliqs</t>
   </si>
   <si>
-    <t>엘리퀴스정2.5mg</t>
-  </si>
-  <si>
-    <t>29</t>
+    <t>30</t>
+  </si>
+  <si>
+    <t>베라스트정 0.02mg</t>
   </si>
   <si>
     <t>bera2</t>
   </si>
   <si>
-    <t>베라스트정 0.02mg</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>46682</t>
   </si>
   <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>리피논정80mg</t>
+  </si>
+  <si>
     <t>lipn8</t>
   </si>
   <si>
-    <t>리피논정80mg</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
     <t>46500</t>
   </si>
   <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>베니톨정</t>
+  </si>
+  <si>
     <t>veni</t>
   </si>
   <si>
-    <t>베니톨정</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
     <t>46591</t>
   </si>
   <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>액시마</t>
+  </si>
+  <si>
     <t>asm</t>
   </si>
   <si>
-    <t>액시마</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
     <t>46902</t>
   </si>
   <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>독시사이클린정100mg</t>
+  </si>
+  <si>
     <t>doxy4</t>
   </si>
   <si>
-    <t>독시사이클린정100mg</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
     <t>46834</t>
   </si>
   <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>베시스타정5mg</t>
+  </si>
+  <si>
     <t>vesi1</t>
   </si>
   <si>
-    <t>베시스타정5mg</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
     <t>46891</t>
   </si>
   <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>듀록타 캡슐 60mg</t>
+  </si>
+  <si>
     <t>duxe60</t>
   </si>
   <si>
-    <t>듀록타 캡슐 60mg</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
     <t>46652</t>
   </si>
   <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>디오반필름코팅정320mg</t>
+  </si>
+  <si>
     <t>dio32</t>
   </si>
   <si>
-    <t>디오반필름코팅정320mg</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
     <t>46630</t>
   </si>
   <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>베아제정</t>
+  </si>
+  <si>
     <t>bease</t>
   </si>
   <si>
-    <t>베아제정</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
     <t>46542</t>
   </si>
   <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>안플라그정100mg</t>
+  </si>
+  <si>
     <t>sapg1</t>
   </si>
   <si>
-    <t>안플라그정100mg</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>46874</t>
   </si>
   <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>치옥티아</t>
+  </si>
+  <si>
     <t>thio-hr1</t>
   </si>
   <si>
-    <t>치옥티아</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
     <t>46562</t>
   </si>
   <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>뮤코테인캡슐</t>
+  </si>
+  <si>
     <t>surf3</t>
   </si>
   <si>
-    <t>뮤코테인캡슐</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
     <t>46661</t>
   </si>
   <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>마이암부톨</t>
+  </si>
+  <si>
     <t>emb1</t>
   </si>
   <si>
-    <t>마이암부톨</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
     <t>46832</t>
   </si>
   <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>산화마그네슘정250mg</t>
+  </si>
+  <si>
     <t>mgo</t>
   </si>
   <si>
-    <t>산화마그네슘정250mg</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
     <t>46480</t>
   </si>
   <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>리바로정2mg</t>
+  </si>
+  <si>
     <t>piva2</t>
   </si>
   <si>
-    <t>리바로정2mg</t>
-  </si>
-  <si>
-    <t>77</t>
+    <t>79</t>
+  </si>
+  <si>
+    <t>비타메진50mg</t>
   </si>
   <si>
     <t>vtm</t>
   </si>
   <si>
-    <t>비타메진50mg</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
     <t>46845</t>
   </si>
   <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>고덱스</t>
+  </si>
+  <si>
     <t>godex</t>
   </si>
   <si>
-    <t>고덱스</t>
-  </si>
-  <si>
-    <t>80</t>
+    <t>81</t>
+  </si>
+  <si>
+    <t>플라빅스에이</t>
   </si>
   <si>
     <t>clpda</t>
   </si>
   <si>
-    <t>플라빅스에이</t>
-  </si>
-  <si>
-    <t>81</t>
+    <t>82</t>
+  </si>
+  <si>
+    <t>아다핀오스서방정30mg</t>
   </si>
   <si>
     <t>nife3</t>
   </si>
   <si>
-    <t>아다핀오스서방정30mg</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
     <t>46191</t>
   </si>
   <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>신일피리독신정</t>
+  </si>
+  <si>
     <t>vb6</t>
   </si>
   <si>
-    <t>신일피리독신정</t>
-  </si>
-  <si>
-    <t>83</t>
+    <t>85</t>
+  </si>
+  <si>
+    <t>아지로신정</t>
   </si>
   <si>
     <t>zim25</t>
   </si>
   <si>
-    <t>아지로신정</t>
-  </si>
-  <si>
-    <t>85</t>
+    <t>86</t>
+  </si>
+  <si>
+    <t>테올란비서방캅셀</t>
   </si>
   <si>
     <t>teol</t>
   </si>
   <si>
-    <t>테올란비서방캅셀</t>
-  </si>
-  <si>
-    <t>86</t>
+    <t>87</t>
+  </si>
+  <si>
+    <t>아세트아미노펜300</t>
   </si>
   <si>
     <t>aap3</t>
   </si>
   <si>
-    <t>아세트아미노펜300</t>
-  </si>
-  <si>
-    <t>87</t>
+    <t>88</t>
+  </si>
+  <si>
+    <t>루키오정10mg</t>
   </si>
   <si>
     <t>sing1</t>
   </si>
   <si>
-    <t>루키오정10mg</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
     <t>46757</t>
   </si>
   <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>노바스크</t>
+  </si>
+  <si>
     <t>nor</t>
   </si>
   <si>
-    <t>노바스크</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
     <t>46399</t>
   </si>
   <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>오팔몬정</t>
+  </si>
+  <si>
     <t>lip</t>
   </si>
   <si>
-    <t>오팔몬정</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
     <t>46856</t>
   </si>
   <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>반코진캡슐125mg</t>
+  </si>
+  <si>
     <t>van</t>
   </si>
   <si>
-    <t>반코진캡슐125mg</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
     <t>46921</t>
   </si>
   <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>애니세프캅셀</t>
+  </si>
+  <si>
     <t>cfd1</t>
   </si>
   <si>
-    <t>애니세프캅셀</t>
-  </si>
-  <si>
-    <t>122</t>
+    <t>123</t>
+  </si>
+  <si>
+    <t>코다론정</t>
   </si>
   <si>
     <t>coda</t>
   </si>
   <si>
-    <t>코다론정</t>
-  </si>
-  <si>
-    <t>123</t>
+    <t>124</t>
+  </si>
+  <si>
+    <t>대원아미노필린정100mg</t>
   </si>
   <si>
     <t>ascta</t>
   </si>
   <si>
-    <t>대원아미노필린정100mg</t>
-  </si>
-  <si>
-    <t>124</t>
+    <t>125</t>
+  </si>
+  <si>
+    <t>아스피린장용정</t>
   </si>
   <si>
     <t>asap</t>
   </si>
   <si>
-    <t>아스피린장용정</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
     <t>46885</t>
   </si>
   <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>디트로딘에스알캡슐4mg</t>
+  </si>
+  <si>
     <t>tfdsr4</t>
   </si>
   <si>
-    <t>디트로딘에스알캡슐4mg</t>
-  </si>
-  <si>
-    <t>127</t>
+    <t>128</t>
+  </si>
+  <si>
+    <t>가바펜틴캡슐 100mg</t>
   </si>
   <si>
     <t>gaba1d</t>
   </si>
   <si>
-    <t>가바펜틴캡슐 100mg</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
     <t>46803</t>
   </si>
   <si>
     <t>gaba1dc</t>
   </si>
   <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>보나링에이</t>
+  </si>
+  <si>
     <t>dmm</t>
   </si>
   <si>
-    <t>보나링에이</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
     <t>46913</t>
   </si>
   <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>아서틸정8mg</t>
+  </si>
+  <si>
     <t>ace8</t>
   </si>
   <si>
-    <t>아서틸정8mg</t>
-  </si>
-  <si>
-    <t>130</t>
+    <t>131</t>
+  </si>
+  <si>
+    <t>에나폰</t>
   </si>
   <si>
     <t>ena</t>
   </si>
   <si>
-    <t>에나폰</t>
-  </si>
-  <si>
-    <t>131</t>
+    <t>133</t>
+  </si>
+  <si>
+    <t>리리카50mg</t>
   </si>
   <si>
     <t>lyri5</t>
   </si>
   <si>
-    <t>리리카50mg</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
     <t>46771</t>
   </si>
   <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>로파인캡슐</t>
+  </si>
+  <si>
     <t>lpr3</t>
   </si>
   <si>
-    <t>로파인캡슐</t>
-  </si>
-  <si>
-    <t>134</t>
+    <t>136</t>
+  </si>
+  <si>
+    <t>오잘탄정50mg</t>
   </si>
   <si>
     <t>lst1</t>
   </si>
   <si>
-    <t>오잘탄정50mg</t>
-  </si>
-  <si>
-    <t>136</t>
+    <t>137</t>
+  </si>
+  <si>
+    <t>비바코정10mg</t>
   </si>
   <si>
     <t>cres3</t>
   </si>
   <si>
-    <t>비바코정10mg</t>
-  </si>
-  <si>
-    <t>137</t>
+    <t>139</t>
+  </si>
+  <si>
+    <t>펙소나딘 정 120mg</t>
   </si>
   <si>
     <t>alle1</t>
   </si>
   <si>
-    <t>펙소나딘 정 120mg</t>
-  </si>
-  <si>
-    <t>139</t>
+    <t>140</t>
+  </si>
+  <si>
+    <t>아프로벨정300mg</t>
   </si>
   <si>
     <t>ibst3</t>
   </si>
   <si>
-    <t>아프로벨정300mg</t>
-  </si>
-  <si>
-    <t>140</t>
+    <t>141</t>
+  </si>
+  <si>
+    <t>부루펜정200mg</t>
   </si>
   <si>
     <t>bf1</t>
   </si>
   <si>
-    <t>부루펜정200mg</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
     <t>47610</t>
   </si>
   <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>리페리돈정0.5mg</t>
+  </si>
+  <si>
     <t>risp0.5</t>
   </si>
   <si>
-    <t>리페리돈정0.5mg</t>
-  </si>
-  <si>
-    <t>142</t>
+    <t>143</t>
+  </si>
+  <si>
+    <t>에이프렉사 정 2.5mg</t>
   </si>
   <si>
     <t>zypr2</t>
   </si>
   <si>
-    <t>에이프렉사 정 2.5mg</t>
-  </si>
-  <si>
-    <t>143</t>
+    <t>145</t>
+  </si>
+  <si>
+    <t>멀택정</t>
   </si>
   <si>
     <t>multac</t>
   </si>
   <si>
-    <t>멀택정</t>
-  </si>
-  <si>
-    <t>145</t>
+    <t>147</t>
+  </si>
+  <si>
+    <t>로수젯정10/10mg</t>
   </si>
   <si>
     <t>crez2</t>
   </si>
   <si>
-    <t>로수젯정10/10mg</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
     <t>46881</t>
   </si>
   <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>유한짓</t>
+  </si>
+  <si>
     <t>inh</t>
   </si>
   <si>
-    <t>유한짓</t>
-  </si>
-  <si>
-    <t>149</t>
+    <t>150</t>
+  </si>
+  <si>
+    <t>신지로이드</t>
   </si>
   <si>
     <t>syn</t>
   </si>
   <si>
-    <t>신지로이드</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
     <t>46895</t>
   </si>
   <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>글리아티린연질캡슐</t>
+  </si>
+  <si>
     <t>glia2</t>
   </si>
   <si>
-    <t>글리아티린연질캡슐</t>
-  </si>
-  <si>
-    <t>182</t>
-  </si>
-  <si>
     <t>46924</t>
   </si>
   <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>글리멜정4mg</t>
+  </si>
+  <si>
     <t>glmd4</t>
   </si>
   <si>
-    <t>글리멜정4mg</t>
-  </si>
-  <si>
-    <t>183</t>
+    <t>184</t>
+  </si>
+  <si>
+    <t>헤르벤</t>
   </si>
   <si>
     <t>herb</t>
   </si>
   <si>
-    <t>헤르벤</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
     <t>46872</t>
   </si>
   <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>레복사신정100mg</t>
+  </si>
+  <si>
     <t>lofx2</t>
   </si>
   <si>
-    <t>레복사신정100mg</t>
-  </si>
-  <si>
-    <t>185</t>
-  </si>
-  <si>
     <t>46701</t>
   </si>
   <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>펙소스타</t>
+  </si>
+  <si>
     <t>fexo</t>
   </si>
   <si>
-    <t>펙소스타</t>
-  </si>
-  <si>
-    <t>188</t>
+    <t>189</t>
+  </si>
+  <si>
+    <t>디아미크롱서방정60mg</t>
   </si>
   <si>
     <t>gc6</t>
   </si>
   <si>
-    <t>디아미크롱서방정60mg</t>
-  </si>
-  <si>
-    <t>189</t>
-  </si>
-  <si>
     <t>46801</t>
   </si>
   <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>아세로</t>
+  </si>
+  <si>
     <t>acl</t>
   </si>
   <si>
-    <t>아세로</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
     <t>46835</t>
   </si>
   <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>릭시아나정30mg</t>
+  </si>
+  <si>
     <t>lixi3</t>
   </si>
   <si>
-    <t>릭시아나정30mg</t>
-  </si>
-  <si>
-    <t>191</t>
-  </si>
-  <si>
     <t>47565</t>
   </si>
   <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>엘리퀴스정5mg</t>
+  </si>
+  <si>
     <t>eliqs5</t>
   </si>
   <si>
-    <t>엘리퀴스정5mg</t>
-  </si>
-  <si>
-    <t>193</t>
+    <t>195</t>
+  </si>
+  <si>
+    <t>훼로바-유서방정</t>
   </si>
   <si>
     <t>fero-u</t>
   </si>
   <si>
-    <t>훼로바-유서방정</t>
-  </si>
-  <si>
-    <t>195</t>
-  </si>
-  <si>
     <t>46912</t>
   </si>
   <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>바스티난서방정</t>
+  </si>
+  <si>
     <t>tmz-mr</t>
   </si>
   <si>
-    <t>바스티난서방정</t>
-  </si>
-  <si>
-    <t>196</t>
-  </si>
-  <si>
     <t>46766</t>
   </si>
   <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>티로파</t>
+  </si>
+  <si>
     <t>tiro</t>
   </si>
   <si>
-    <t>티로파</t>
-  </si>
-  <si>
-    <t>197</t>
-  </si>
-  <si>
     <t>47644</t>
   </si>
   <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>팜시버 정 250mg</t>
+  </si>
+  <si>
     <t>famcv1</t>
   </si>
   <si>
-    <t>팜시버 정 250mg</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
     <t>46854</t>
   </si>
   <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>유니네콜정25mg</t>
+  </si>
+  <si>
     <t>btc25</t>
   </si>
   <si>
-    <t>유니네콜정25mg</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
     <t>46889</t>
   </si>
   <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>가스터디정</t>
+  </si>
+  <si>
     <t>gstd</t>
   </si>
   <si>
-    <t>가스터디정</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
     <t>46752</t>
   </si>
   <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>빔스크정100mg</t>
+  </si>
+  <si>
     <t>lacosa1</t>
   </si>
   <si>
-    <t>빔스크정100mg</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
     <t>46694</t>
   </si>
   <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>오로살탄5/80</t>
+  </si>
+  <si>
     <t>orsal</t>
   </si>
   <si>
-    <t>오로살탄5/80</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
     <t>46906</t>
   </si>
   <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>탐스오디정</t>
+  </si>
+  <si>
     <t>har-d1</t>
   </si>
   <si>
-    <t>탐스오디정</t>
-  </si>
-  <si>
-    <t>209</t>
+    <t>210</t>
+  </si>
+  <si>
+    <t>피나스테리드정5mg</t>
   </si>
   <si>
     <t>pros3</t>
   </si>
   <si>
-    <t>피나스테리드정5mg</t>
-  </si>
-  <si>
-    <t>210</t>
-  </si>
-  <si>
     <t>46481</t>
   </si>
   <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>노르믹스정</t>
+  </si>
+  <si>
     <t>nrmx</t>
   </si>
   <si>
-    <t>노르믹스정</t>
-  </si>
-  <si>
-    <t>213</t>
-  </si>
-  <si>
     <t>46886</t>
   </si>
   <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>스피로닥톤정25mg</t>
+  </si>
+  <si>
     <t>spr</t>
   </si>
   <si>
-    <t>스피로닥톤정25mg</t>
-  </si>
-  <si>
-    <t>214</t>
-  </si>
-  <si>
     <t>46948</t>
   </si>
   <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>엔테론정150mg</t>
+  </si>
+  <si>
     <t>ent</t>
   </si>
   <si>
-    <t>엔테론정150mg</t>
-  </si>
-  <si>
-    <t>215</t>
+    <t>216</t>
+  </si>
+  <si>
+    <t>비유피-4정20mg</t>
   </si>
   <si>
     <t>ppv</t>
   </si>
   <si>
-    <t>비유피-4정20mg</t>
-  </si>
-  <si>
-    <t>216</t>
+    <t>219</t>
+  </si>
+  <si>
+    <t>셉트린정</t>
   </si>
   <si>
     <t>ts1</t>
   </si>
   <si>
-    <t>셉트린정</t>
-  </si>
-  <si>
-    <t>219</t>
+    <t>220</t>
+  </si>
+  <si>
+    <t>액티피드</t>
   </si>
   <si>
     <t>afdj</t>
   </si>
   <si>
-    <t>액티피드</t>
-  </si>
-  <si>
-    <t>220</t>
+    <t>221</t>
+  </si>
+  <si>
+    <t>디오살탄정80mg</t>
   </si>
   <si>
     <t>dio80</t>
   </si>
   <si>
-    <t>디오살탄정80mg</t>
-  </si>
-  <si>
-    <t>221</t>
-  </si>
-  <si>
     <t>46933</t>
   </si>
   <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>코프렐</t>
+  </si>
+  <si>
     <t>cof</t>
   </si>
   <si>
-    <t>코프렐</t>
-  </si>
-  <si>
-    <t>222</t>
+    <t>225</t>
+  </si>
+  <si>
+    <t>자디앙정25mg</t>
   </si>
   <si>
     <t>jard1</t>
   </si>
   <si>
-    <t>자디앙정25mg</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
     <t>46691</t>
   </si>
   <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>다파엔정10mg</t>
+  </si>
+  <si>
     <t>foxig1</t>
   </si>
   <si>
-    <t>다파엔정10mg</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
     <t>46947</t>
   </si>
   <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>아리페질정</t>
+  </si>
+  <si>
     <t>dnpz5</t>
   </si>
   <si>
-    <t>아리페질정</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
     <t>46506</t>
   </si>
   <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>릭시아나정15mg</t>
+  </si>
+  <si>
     <t>lixi15</t>
-  </si>
-  <si>
-    <t>릭시아나정15mg</t>
-  </si>
-  <si>
-    <t>228</t>
   </si>
 </sst>
 </file>
@@ -1574,10 +1574,9 @@
   <dimension ref="A1:D27"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="3" max="4" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,10 +1968,9 @@
   <dimension ref="A1:D26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="3" max="4" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,10 +2348,9 @@
   <dimension ref="A1:D25"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="3" max="4" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2470,13 +2467,13 @@
     </row>
     <row r="9" ht="18" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>212</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>214</v>
@@ -2717,10 +2714,9 @@
   <dimension ref="A1:D32"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="3" max="4" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>